<commit_message>
Updated experiment Lx with new observations
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Lx_Parameters_Estimation/0-Dataset/LX_OBS_WITH_FEATURES.xlsx
+++ b/Parameters-Estimation/Lx_Parameters_Estimation/0-Dataset/LX_OBS_WITH_FEATURES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\4_Estuarine Box Model\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_Estuarine Box Model\Experiments\Parameters-Estimation\Lx_Parameters_Estimation\0-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975C021D-ED44-434E-933A-300EE0247B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF1030D-61D9-4371-B5F8-40147298C460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4455" windowWidth="20730" windowHeight="11160" xr2:uid="{C0F15CBA-0785-B24A-A131-C199A94A0422}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0F15CBA-0785-B24A-A131-C199A94A0422}"/>
   </bookViews>
   <sheets>
     <sheet name="Lx_obs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t>DATE</t>
   </si>
@@ -52,16 +52,19 @@
     <t>Q_tide</t>
   </si>
   <si>
-    <t xml:space="preserve">Lx OBS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATION RANGE </t>
-  </si>
-  <si>
     <t>Dataset_Type</t>
   </si>
   <si>
     <t>CALIBRATION RANGE</t>
+  </si>
+  <si>
+    <t>VALIDATION RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lx_OBS </t>
+  </si>
+  <si>
+    <t>Lx_Model</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,6 +156,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E358E3-1251-0342-BD56-025EC52DDF8A}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -481,10 +487,11 @@
     <col min="4" max="4" width="10.875" style="10"/>
     <col min="5" max="5" width="11" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25">
+    <row r="1" spans="1:8" ht="26.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,13 +508,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="26.25">
+    </row>
+    <row r="2" spans="1:8" ht="26.25">
       <c r="A2" s="5">
         <v>37803</v>
       </c>
@@ -526,11 +536,14 @@
       <c r="F2" s="7">
         <v>14.3</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="26.25">
+      <c r="G2" s="13">
+        <v>12.2</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="26.25">
       <c r="A3" s="5">
         <v>37826</v>
       </c>
@@ -549,11 +562,14 @@
       <c r="F3" s="7">
         <v>26.7</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="26.25">
+      <c r="G3" s="13">
+        <v>17.7</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="26.25">
       <c r="A4" s="5">
         <v>37866</v>
       </c>
@@ -572,11 +588,14 @@
       <c r="F4" s="7">
         <v>13</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="26.25">
+      <c r="G4" s="13">
+        <v>9.5</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="26.25">
       <c r="A5" s="5">
         <v>38166</v>
       </c>
@@ -595,11 +614,14 @@
       <c r="F5" s="7">
         <v>12.4</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="26.25">
+      <c r="G5" s="13">
+        <v>10.6</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="26.25">
       <c r="A6" s="5">
         <v>38392</v>
       </c>
@@ -618,11 +640,14 @@
       <c r="F6" s="7">
         <v>11.9</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="26.25">
+      <c r="G6" s="13">
+        <v>12</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="26.25">
       <c r="A7" s="5">
         <v>38531</v>
       </c>
@@ -641,11 +666,14 @@
       <c r="F7" s="7">
         <v>20.5</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="26.25">
+      <c r="G7" s="13">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="26.25">
       <c r="A8" s="5">
         <v>38589</v>
       </c>
@@ -664,11 +692,14 @@
       <c r="F8" s="7">
         <v>10.6</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="26.25">
+      <c r="G8" s="13">
+        <v>9.5</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="26.25">
       <c r="A9" s="5">
         <v>38897</v>
       </c>
@@ -687,11 +718,14 @@
       <c r="F9" s="7">
         <v>26</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="26.25">
+      <c r="G9" s="13">
+        <v>20.3</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="26.25">
       <c r="A10" s="5">
         <v>39016</v>
       </c>
@@ -710,11 +744,14 @@
       <c r="F10" s="7">
         <v>5.8</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="26.25">
+      <c r="G10" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="26.25">
       <c r="A11" s="5">
         <v>39184</v>
       </c>
@@ -733,11 +770,14 @@
       <c r="F11" s="7">
         <v>13.1</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="26.25">
+      <c r="G11" s="13">
+        <v>10.9</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="26.25">
       <c r="A12" s="5">
         <v>39297</v>
       </c>
@@ -756,11 +796,14 @@
       <c r="F12" s="7">
         <v>15.3</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="26.25">
+      <c r="G12" s="13">
+        <v>15.5</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="26.25">
       <c r="A13" s="5">
         <v>39728</v>
       </c>
@@ -779,11 +822,14 @@
       <c r="F13" s="7">
         <v>13.2</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="26.25">
+      <c r="G13" s="13">
+        <v>7.6</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="26.25">
       <c r="A14" s="5">
         <v>39898</v>
       </c>
@@ -802,11 +848,14 @@
       <c r="F14" s="7">
         <v>4.7</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="26.25">
+      <c r="G14" s="13">
+        <v>8.4</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="26.25">
       <c r="A15" s="5">
         <v>40001</v>
       </c>
@@ -825,11 +874,14 @@
       <c r="F15" s="7">
         <v>6.7</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="26.25">
+      <c r="G15" s="13">
+        <v>7.7</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="26.25">
       <c r="A16" s="5">
         <v>40022</v>
       </c>
@@ -848,11 +900,14 @@
       <c r="F16" s="7">
         <v>12.2</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="26.25">
+      <c r="G16" s="13">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="26.25">
       <c r="A17" s="5">
         <v>40050</v>
       </c>
@@ -871,11 +926,14 @@
       <c r="F17" s="7">
         <v>12.5</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="26.25">
+      <c r="G17" s="13">
+        <v>9.4</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="26.25">
       <c r="A18" s="5">
         <v>40115</v>
       </c>
@@ -894,11 +952,14 @@
       <c r="F18" s="7">
         <v>12</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="26.25">
+      <c r="G18" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="26.25">
       <c r="A19" s="5">
         <v>40381</v>
       </c>
@@ -917,11 +978,14 @@
       <c r="F19" s="7">
         <v>16.100000000000001</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="26.25">
+      <c r="G19" s="13">
+        <v>10.8</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="26.25">
       <c r="A20" s="5">
         <v>40737</v>
       </c>
@@ -940,11 +1004,14 @@
       <c r="F20" s="7">
         <v>15</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="26.25">
+      <c r="G20" s="13">
+        <v>12.1</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="26.25">
       <c r="A21" s="5">
         <v>41130</v>
       </c>
@@ -963,11 +1030,14 @@
       <c r="F21" s="7">
         <v>20.6</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="26.25">
+      <c r="G21" s="13">
+        <v>10.6</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="26.25">
       <c r="A22" s="5">
         <v>41499</v>
       </c>
@@ -986,11 +1056,14 @@
       <c r="F22" s="7">
         <v>8.3000000000000007</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="26.25">
+      <c r="G22" s="13">
+        <v>6.4</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="26.25">
       <c r="A23" s="5">
         <v>42208</v>
       </c>
@@ -1009,11 +1082,14 @@
       <c r="F23" s="7">
         <v>18.5</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="26.25">
+      <c r="G23" s="13">
+        <v>10.7</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="26.25">
       <c r="A24" s="5">
         <v>42606</v>
       </c>
@@ -1032,11 +1108,14 @@
       <c r="F24" s="7">
         <v>12.6</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="26.25">
+      <c r="G24" s="13">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="26.25">
       <c r="A25" s="5">
         <v>42914</v>
       </c>
@@ -1055,11 +1134,14 @@
       <c r="F25" s="7">
         <v>11.5</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="26.25">
+      <c r="G25" s="13">
+        <v>12.6</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="26.25">
       <c r="A26" s="5">
         <v>42948</v>
       </c>
@@ -1078,36 +1160,147 @@
       <c r="F26" s="7">
         <v>20</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="26.25">
-      <c r="A27" s="5"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" ht="26.25">
-      <c r="A28" s="5"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" ht="26.25">
-      <c r="A29" s="5"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" ht="26.25">
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" ht="26.25">
-      <c r="A31" s="5"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="26.25">
-      <c r="A32" s="5"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" ht="26.25">
-      <c r="A33" s="5"/>
-      <c r="F33" s="7"/>
+      <c r="G26" s="13">
+        <v>10.6</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q26" s="13"/>
+    </row>
+    <row r="27" spans="1:17" ht="26.25">
+      <c r="A27" s="5">
+        <v>38019</v>
+      </c>
+      <c r="B27" s="6">
+        <v>2.91</v>
+      </c>
+      <c r="C27" s="7">
+        <v>86.1</v>
+      </c>
+      <c r="D27" s="6">
+        <v>36.82</v>
+      </c>
+      <c r="E27" s="6">
+        <v>17.38</v>
+      </c>
+      <c r="F27" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="G27" s="13">
+        <v>9.1</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="13"/>
+    </row>
+    <row r="28" spans="1:17" ht="26.25">
+      <c r="A28" s="5">
+        <v>38482</v>
+      </c>
+      <c r="B28" s="6">
+        <v>18.16</v>
+      </c>
+      <c r="C28" s="7">
+        <v>90.4</v>
+      </c>
+      <c r="D28" s="6">
+        <v>36.31</v>
+      </c>
+      <c r="E28" s="6">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="F28" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G28" s="13">
+        <v>7.9</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:17" ht="26.25">
+      <c r="A29" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="C29" s="7">
+        <v>270</v>
+      </c>
+      <c r="D29" s="6">
+        <v>37.28</v>
+      </c>
+      <c r="E29" s="6">
+        <v>11.7</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G29" s="7">
+        <v>5</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="13"/>
+    </row>
+    <row r="30" spans="1:17" ht="26.25">
+      <c r="A30" s="5">
+        <v>40255</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="C30" s="7">
+        <v>162.30000000000001</v>
+      </c>
+      <c r="D30" s="6">
+        <v>38.17</v>
+      </c>
+      <c r="E30" s="6">
+        <v>19.3</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="G30" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q30" s="13"/>
+    </row>
+    <row r="31" spans="1:17" ht="26.25">
+      <c r="A31" s="5">
+        <v>40332</v>
+      </c>
+      <c r="B31" s="6">
+        <v>3.03</v>
+      </c>
+      <c r="C31" s="7">
+        <v>189.6</v>
+      </c>
+      <c r="D31" s="6">
+        <v>36.75</v>
+      </c>
+      <c r="E31" s="6">
+        <v>14.3</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G31" s="13">
+        <v>5.7</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="26.25">
       <c r="A34" s="5"/>

</xml_diff>